<commit_message>
Implemented code for generating data with pMEDICI
</commit_message>
<xml_diff>
--- a/pMEDICI/experimentData/pMEDICI_Generation_from_scratch.xlsx
+++ b/pMEDICI/experimentData/pMEDICI_Generation_from_scratch.xlsx
@@ -6,13 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ACTS_Generation_from_scratch" r:id="rId3" sheetId="1"/>
+    <sheet name="TIME (ms) for generating TS" r:id="rId3" sheetId="1"/>
+    <sheet name="SIZE of the generated TS" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>AmbientAssistedLivingv1</t>
   </si>
@@ -161,7 +162,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:AJ2"/>
+  <dimension ref="B2:AJ4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -274,6 +275,554 @@
         <v>34</v>
       </c>
     </row>
+    <row r="3">
+      <c r="B3" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>38.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>35.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="B2:AJ4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" t="s">
+        <v>19</v>
+      </c>
+      <c r="V2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>24.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>